<commit_message>
fix the bug of index
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10524"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlk/Desktop/Artificial Intelligence/3rd Year/Bayesian Networks/week3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCBFA25-027A-254D-9534-E460F4442C08}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F31E8B-383F-CA4F-81C1-A154D73A2929}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{DB84CAA0-3DCF-CB46-8FAD-DB5DD16BECCF}"/>
   </bookViews>
@@ -612,10 +612,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>120</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3957,8 +3957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D3DAD7-F3E9-6843-AA1F-1023F35B349C}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -4414,7 +4414,7 @@
         <v>2</v>
       </c>
       <c r="C55" s="8">
-        <v>0</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -4425,7 +4425,7 @@
         <v>20</v>
       </c>
       <c r="C56" s="8">
-        <v>120</v>
+        <v>72</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>